<commit_message>
Minor changes in file
mostly column formatting
</commit_message>
<xml_diff>
--- a/AGRC_PGROUP_MATCH.xlsx
+++ b/AGRC_PGROUP_MATCH.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="AGRC" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">AGRC!$A$1:$C$1283</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -8601,8 +8604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G299" sqref="G299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>